<commit_message>
Added various things that were lying around
</commit_message>
<xml_diff>
--- a/cambridge/elections/2017/locals/projection/projected.xlsx
+++ b/cambridge/elections/2017/locals/projection/projected.xlsx
@@ -14,9 +14,6 @@
   <sheets>
     <sheet name="projected" sheetId="1" r:id="rId1"/>
   </sheets>
-  <externalReferences>
-    <externalReference r:id="rId2"/>
-  </externalReferences>
   <calcPr calcId="0" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
@@ -139,9 +136,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -542,11 +541,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-1781801072"/>
-        <c:axId val="-1781798512"/>
+        <c:axId val="1846871936"/>
+        <c:axId val="1846874512"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-1781801072"/>
+        <c:axId val="1846871936"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -556,7 +555,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-1781798512"/>
+        <c:crossAx val="1846874512"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -564,7 +563,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1781798512"/>
+        <c:axId val="1846874512"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="0.7"/>
@@ -576,7 +575,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-1781801072"/>
+        <c:crossAx val="1846871936"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -650,7 +649,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -1141,11 +1139,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-1661839664"/>
-        <c:axId val="-1662187696"/>
+        <c:axId val="1847797104"/>
+        <c:axId val="1847799584"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-1661839664"/>
+        <c:axId val="1847797104"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1155,7 +1153,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-1662187696"/>
+        <c:crossAx val="1847799584"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1163,7 +1161,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1662187696"/>
+        <c:axId val="1847799584"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="0.5"/>
@@ -1175,7 +1173,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-1661839664"/>
+        <c:crossAx val="1847797104"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="0.1"/>
@@ -1183,7 +1181,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -1824,11 +1821,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-1663498784"/>
-        <c:axId val="-1663981360"/>
+        <c:axId val="1847843264"/>
+        <c:axId val="1847845744"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-1663498784"/>
+        <c:axId val="1847843264"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1838,7 +1835,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-1663981360"/>
+        <c:crossAx val="1847845744"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1846,7 +1843,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1663981360"/>
+        <c:axId val="1847845744"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="0.6"/>
@@ -1858,7 +1855,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-1663498784"/>
+        <c:crossAx val="1847843264"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="0.1"/>
@@ -1998,19 +1995,19 @@
                 <c:formatCode>0.0%</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>0.187774524158125</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.136123680241327</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.163227016885553</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0.245287253141831</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0.196673897324656</c:v>
+                  <c:v>0.327897218236407</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.311796007829623</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.268738524678691</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.268574943127425</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.221543176020963</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2082,19 +2079,19 @@
                 <c:formatCode>0.0%</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>0.0629575402635431</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.0648567119155354</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.113508442776735</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0.122531418312387</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0.0838756326825741</c:v>
+                  <c:v>0.127681381356034</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.104387167856347</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.148652662274543</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.145820251783379</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.100751303681649</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2166,19 +2163,19 @@
                 <c:formatCode>0.0%</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>0.396778916544655</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.351055806938159</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.297373358348968</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0.247307001795332</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0.289587852494577</c:v>
+                  <c:v>0.212689761614797</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.198184418111279</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.186318716924073</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.237624424840705</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.262229360913056</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2250,19 +2247,19 @@
                 <c:formatCode>0.0%</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>0.352489019033674</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.447963800904977</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.425891181988743</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0.337073608617594</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0.429862617498192</c:v>
+                  <c:v>0.33173163879276</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.385632406202749</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.396290096122691</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.304677447579441</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.415476159384331</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2333,7 +2330,7 @@
                 <c:formatCode>0.0%</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="3">
-                  <c:v>0.0478007181328545</c:v>
+                  <c:v>0.0433029326690479</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2350,11 +2347,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-1664379056"/>
-        <c:axId val="-1744037840"/>
+        <c:axId val="1847879872"/>
+        <c:axId val="1847882352"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-1664379056"/>
+        <c:axId val="1847879872"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2364,7 +2361,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-1744037840"/>
+        <c:crossAx val="1847882352"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2372,7 +2369,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1744037840"/>
+        <c:axId val="1847882352"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="0.5"/>
@@ -2384,7 +2381,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-1664379056"/>
+        <c:crossAx val="1847879872"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="0.1"/>
@@ -2976,11 +2973,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-1740964448"/>
-        <c:axId val="-1705974160"/>
+        <c:axId val="1846905520"/>
+        <c:axId val="1846908000"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-1740964448"/>
+        <c:axId val="1846905520"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2990,7 +2987,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-1705974160"/>
+        <c:crossAx val="1846908000"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2998,7 +2995,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1705974160"/>
+        <c:axId val="1846908000"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="0.6"/>
@@ -3010,7 +3007,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-1740964448"/>
+        <c:crossAx val="1846905520"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3598,11 +3595,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-1738297680"/>
-        <c:axId val="-1668118688"/>
+        <c:axId val="1846951680"/>
+        <c:axId val="1846954160"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-1738297680"/>
+        <c:axId val="1846951680"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3612,7 +3609,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-1668118688"/>
+        <c:crossAx val="1846954160"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3620,7 +3617,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1668118688"/>
+        <c:axId val="1846954160"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="0.5"/>
@@ -3632,7 +3629,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-1738297680"/>
+        <c:crossAx val="1846951680"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="0.1"/>
@@ -4205,11 +4202,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-1667328432"/>
-        <c:axId val="-1667327072"/>
+        <c:axId val="1846994064"/>
+        <c:axId val="1846996544"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-1667328432"/>
+        <c:axId val="1846994064"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4219,7 +4216,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-1667327072"/>
+        <c:crossAx val="1846996544"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4227,7 +4224,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1667327072"/>
+        <c:axId val="1846996544"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="0.7"/>
@@ -4239,7 +4236,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-1667328432"/>
+        <c:crossAx val="1846994064"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="0.1"/>
@@ -4743,11 +4740,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-1705543264"/>
-        <c:axId val="-1667905536"/>
+        <c:axId val="1847029520"/>
+        <c:axId val="1847032000"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-1705543264"/>
+        <c:axId val="1847029520"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4757,7 +4754,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-1667905536"/>
+        <c:crossAx val="1847032000"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4765,7 +4762,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1667905536"/>
+        <c:axId val="1847032000"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="0.5"/>
@@ -4777,7 +4774,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-1705543264"/>
+        <c:crossAx val="1847029520"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="0.1"/>
@@ -5374,11 +5371,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-1665003424"/>
-        <c:axId val="-1664594032"/>
+        <c:axId val="1847074368"/>
+        <c:axId val="1847076848"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-1665003424"/>
+        <c:axId val="1847074368"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5388,7 +5385,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-1664594032"/>
+        <c:crossAx val="1847076848"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -5396,7 +5393,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1664594032"/>
+        <c:axId val="1847076848"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="0.6"/>
@@ -5408,7 +5405,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-1665003424"/>
+        <c:crossAx val="1847074368"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="0.1"/>
@@ -5986,11 +5983,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-1664810800"/>
-        <c:axId val="-1664144336"/>
+        <c:axId val="1847116352"/>
+        <c:axId val="1847118832"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-1664810800"/>
+        <c:axId val="1847116352"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6000,7 +5997,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-1664144336"/>
+        <c:crossAx val="1847118832"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -6008,7 +6005,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1664144336"/>
+        <c:axId val="1847118832"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="0.5"/>
@@ -6020,7 +6017,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-1664810800"/>
+        <c:crossAx val="1847116352"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="0.1"/>
@@ -6596,11 +6593,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-1780858320"/>
-        <c:axId val="-1662488096"/>
+        <c:axId val="1847711776"/>
+        <c:axId val="1847714256"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-1780858320"/>
+        <c:axId val="1847711776"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6610,7 +6607,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-1662488096"/>
+        <c:crossAx val="1847714256"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -6618,7 +6615,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1662488096"/>
+        <c:axId val="1847714256"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="0.5"/>
@@ -6630,7 +6627,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-1780858320"/>
+        <c:crossAx val="1847711776"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="0.1"/>
@@ -6705,7 +6702,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -7124,11 +7120,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-1665007344"/>
-        <c:axId val="-1664137680"/>
+        <c:axId val="1847755520"/>
+        <c:axId val="1847758000"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-1665007344"/>
+        <c:axId val="1847755520"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7138,7 +7134,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-1664137680"/>
+        <c:crossAx val="1847758000"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -7146,7 +7142,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1664137680"/>
+        <c:axId val="1847758000"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="0.6"/>
@@ -7158,7 +7154,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-1665007344"/>
+        <c:crossAx val="1847755520"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="0.1"/>
@@ -7166,7 +7162,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -7198,13 +7193,13 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>8</xdr:col>
+      <xdr:col>9</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>2</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>17</xdr:col>
+      <xdr:col>18</xdr:col>
       <xdr:colOff>88900</xdr:colOff>
       <xdr:row>23</xdr:row>
       <xdr:rowOff>63500</xdr:rowOff>
@@ -7230,13 +7225,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>18</xdr:col>
+      <xdr:col>19</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>2</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>27</xdr:col>
+      <xdr:col>28</xdr:col>
       <xdr:colOff>88900</xdr:colOff>
       <xdr:row>23</xdr:row>
       <xdr:rowOff>63500</xdr:rowOff>
@@ -7262,13 +7257,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>8</xdr:col>
+      <xdr:col>9</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>24</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>17</xdr:col>
+      <xdr:col>18</xdr:col>
       <xdr:colOff>88900</xdr:colOff>
       <xdr:row>45</xdr:row>
       <xdr:rowOff>63500</xdr:rowOff>
@@ -7294,13 +7289,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>18</xdr:col>
+      <xdr:col>19</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>24</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>27</xdr:col>
+      <xdr:col>28</xdr:col>
       <xdr:colOff>88900</xdr:colOff>
       <xdr:row>45</xdr:row>
       <xdr:rowOff>63500</xdr:rowOff>
@@ -7326,13 +7321,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>8</xdr:col>
+      <xdr:col>9</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>47</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>17</xdr:col>
+      <xdr:col>18</xdr:col>
       <xdr:colOff>88900</xdr:colOff>
       <xdr:row>68</xdr:row>
       <xdr:rowOff>63500</xdr:rowOff>
@@ -7358,13 +7353,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>18</xdr:col>
+      <xdr:col>19</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>47</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>27</xdr:col>
+      <xdr:col>28</xdr:col>
       <xdr:colOff>88900</xdr:colOff>
       <xdr:row>68</xdr:row>
       <xdr:rowOff>63500</xdr:rowOff>
@@ -7390,13 +7385,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>8</xdr:col>
+      <xdr:col>9</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>70</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>17</xdr:col>
+      <xdr:col>18</xdr:col>
       <xdr:colOff>88900</xdr:colOff>
       <xdr:row>91</xdr:row>
       <xdr:rowOff>63500</xdr:rowOff>
@@ -7422,13 +7417,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>18</xdr:col>
+      <xdr:col>19</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>69</xdr:row>
       <xdr:rowOff>165100</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>27</xdr:col>
+      <xdr:col>28</xdr:col>
       <xdr:colOff>88900</xdr:colOff>
       <xdr:row>91</xdr:row>
       <xdr:rowOff>25400</xdr:rowOff>
@@ -7454,13 +7449,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>8</xdr:col>
+      <xdr:col>9</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>93</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>17</xdr:col>
+      <xdr:col>18</xdr:col>
       <xdr:colOff>88900</xdr:colOff>
       <xdr:row>114</xdr:row>
       <xdr:rowOff>63500</xdr:rowOff>
@@ -7486,13 +7481,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>18</xdr:col>
+      <xdr:col>19</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>93</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>27</xdr:col>
+      <xdr:col>28</xdr:col>
       <xdr:colOff>88900</xdr:colOff>
       <xdr:row>114</xdr:row>
       <xdr:rowOff>63500</xdr:rowOff>
@@ -7518,13 +7513,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>8</xdr:col>
+      <xdr:col>9</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>116</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>17</xdr:col>
+      <xdr:col>18</xdr:col>
       <xdr:colOff>88900</xdr:colOff>
       <xdr:row>137</xdr:row>
       <xdr:rowOff>63500</xdr:rowOff>
@@ -7550,13 +7545,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>18</xdr:col>
+      <xdr:col>19</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>116</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>27</xdr:col>
+      <xdr:col>28</xdr:col>
       <xdr:colOff>88900</xdr:colOff>
       <xdr:row>137</xdr:row>
       <xdr:rowOff>63500</xdr:rowOff>
@@ -7581,183 +7576,6 @@
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
-</file>
-
-<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <sheetNames>
-      <sheetName val="Sheet1"/>
-      <sheetName val="Sheet2"/>
-      <sheetName val="Sheet4"/>
-      <sheetName val="Sheet5"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0"/>
-      <sheetData sheetId="1"/>
-      <sheetData sheetId="2"/>
-      <sheetData sheetId="3">
-        <row r="1">
-          <cell r="C1">
-            <v>2006</v>
-          </cell>
-          <cell r="D1">
-            <v>2007</v>
-          </cell>
-          <cell r="E1">
-            <v>2008</v>
-          </cell>
-          <cell r="F1">
-            <v>2009</v>
-          </cell>
-          <cell r="G1">
-            <v>2010</v>
-          </cell>
-          <cell r="H1">
-            <v>2011</v>
-          </cell>
-          <cell r="I1">
-            <v>2012</v>
-          </cell>
-          <cell r="J1">
-            <v>2013</v>
-          </cell>
-          <cell r="K1">
-            <v>2014</v>
-          </cell>
-        </row>
-        <row r="68">
-          <cell r="B68" t="str">
-            <v>Con</v>
-          </cell>
-          <cell r="C68">
-            <v>0.20799999999999999</v>
-          </cell>
-          <cell r="D68">
-            <v>0.22900000000000001</v>
-          </cell>
-          <cell r="E68">
-            <v>0.22900000000000001</v>
-          </cell>
-          <cell r="F68">
-            <v>0.20599999999999999</v>
-          </cell>
-          <cell r="G68">
-            <v>0.16044378066993811</v>
-          </cell>
-          <cell r="H68">
-            <v>0.18099999999999999</v>
-          </cell>
-          <cell r="I68">
-            <v>0.16300000000000001</v>
-          </cell>
-          <cell r="J68">
-            <v>0.13200000000000001</v>
-          </cell>
-          <cell r="K68">
-            <v>0.108</v>
-          </cell>
-        </row>
-        <row r="69">
-          <cell r="B69" t="str">
-            <v>Green</v>
-          </cell>
-          <cell r="C69">
-            <v>0.17899999999999999</v>
-          </cell>
-          <cell r="D69">
-            <v>0.16700000000000001</v>
-          </cell>
-          <cell r="E69">
-            <v>0.13500000000000001</v>
-          </cell>
-          <cell r="F69">
-            <v>0.18099999999999999</v>
-          </cell>
-          <cell r="G69">
-            <v>0.2562406656710049</v>
-          </cell>
-          <cell r="H69">
-            <v>0.161</v>
-          </cell>
-          <cell r="I69">
-            <v>0.14199999999999999</v>
-          </cell>
-          <cell r="J69">
-            <v>8.3000000000000004E-2</v>
-          </cell>
-          <cell r="K69">
-            <v>0.106</v>
-          </cell>
-        </row>
-        <row r="70">
-          <cell r="B70" t="str">
-            <v>Lab</v>
-          </cell>
-          <cell r="C70">
-            <v>0.188</v>
-          </cell>
-          <cell r="D70">
-            <v>0.20399999999999999</v>
-          </cell>
-          <cell r="E70">
-            <v>0.20499999999999999</v>
-          </cell>
-          <cell r="F70">
-            <v>0.156</v>
-          </cell>
-          <cell r="G70">
-            <v>0.18199274589289524</v>
-          </cell>
-          <cell r="H70">
-            <v>0.27200000000000002</v>
-          </cell>
-          <cell r="I70">
-            <v>0.32800000000000001</v>
-          </cell>
-          <cell r="J70">
-            <v>0.40899999999999997</v>
-          </cell>
-          <cell r="K70">
-            <v>0.39</v>
-          </cell>
-        </row>
-        <row r="71">
-          <cell r="B71" t="str">
-            <v>Lib Dem</v>
-          </cell>
-          <cell r="C71">
-            <v>0.42499999999999999</v>
-          </cell>
-          <cell r="D71">
-            <v>0.4</v>
-          </cell>
-          <cell r="E71">
-            <v>0.432</v>
-          </cell>
-          <cell r="F71">
-            <v>0.45700000000000002</v>
-          </cell>
-          <cell r="G71">
-            <v>0.40132280776616175</v>
-          </cell>
-          <cell r="H71">
-            <v>0.38500000000000001</v>
-          </cell>
-          <cell r="I71">
-            <v>0.36699999999999999</v>
-          </cell>
-          <cell r="J71">
-            <v>0.376</v>
-          </cell>
-          <cell r="K71">
-            <v>0.39600000000000002</v>
-          </cell>
-        </row>
-      </sheetData>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -8023,15 +7841,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G69"/>
+  <dimension ref="A1:I71"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="L107" workbookViewId="0">
-      <selection activeCell="D27" sqref="D27"/>
+    <sheetView tabSelected="1" topLeftCell="A36" workbookViewId="0">
+      <selection activeCell="H71" sqref="H71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -8053,8 +7871,11 @@
       <c r="G1">
         <v>2016</v>
       </c>
+      <c r="H1">
+        <v>2017</v>
+      </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -8076,8 +7897,9 @@
       <c r="G2" s="1">
         <v>0.11017369727047099</v>
       </c>
+      <c r="H2" s="1"/>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -8099,8 +7921,9 @@
       <c r="G3" s="1">
         <v>0.14491315136476399</v>
       </c>
+      <c r="H3" s="1"/>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -8122,8 +7945,9 @@
       <c r="G4" s="1">
         <v>0.61290322580645096</v>
       </c>
+      <c r="H4" s="1"/>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>2</v>
       </c>
@@ -8145,8 +7969,9 @@
       <c r="G5" s="1">
         <v>0.13200992555831201</v>
       </c>
+      <c r="H5" s="1"/>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>6</v>
       </c>
@@ -8168,8 +7993,9 @@
       <c r="G6" s="1">
         <v>0.108782025984773</v>
       </c>
+      <c r="H6" s="1"/>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -8191,8 +8017,9 @@
       <c r="G7" s="1">
         <v>9.8720684753581395E-2</v>
       </c>
+      <c r="H7" s="1"/>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -8214,8 +8041,9 @@
       <c r="G8" s="1">
         <v>2.9731914681665399E-2</v>
       </c>
+      <c r="H8" s="1"/>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>6</v>
       </c>
@@ -8237,8 +8065,9 @@
       <c r="G9" s="1">
         <v>0.56747727002785397</v>
       </c>
+      <c r="H9" s="1"/>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>6</v>
       </c>
@@ -8260,8 +8089,9 @@
       <c r="G10" s="1">
         <v>0.18845666075348899</v>
       </c>
+      <c r="H10" s="1"/>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>6</v>
       </c>
@@ -8277,8 +8107,9 @@
       <c r="G11" s="1">
         <v>6.8314437986352399E-3</v>
       </c>
+      <c r="H11" s="1"/>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>9</v>
       </c>
@@ -8300,8 +8131,9 @@
       <c r="G12" s="1">
         <v>7.1191011664252499E-2</v>
       </c>
+      <c r="H12" s="1"/>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>9</v>
       </c>
@@ -8323,8 +8155,9 @@
       <c r="G13" s="1">
         <v>8.7086414576503707E-2</v>
       </c>
+      <c r="H13" s="1"/>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>9</v>
       </c>
@@ -8343,8 +8176,9 @@
       <c r="G14" s="1">
         <v>0.210757032858123</v>
       </c>
+      <c r="H14" s="1"/>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>9</v>
       </c>
@@ -8366,8 +8200,9 @@
       <c r="G15" s="1">
         <v>0.38306205687276002</v>
       </c>
+      <c r="H15" s="1"/>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>9</v>
       </c>
@@ -8389,8 +8224,9 @@
       <c r="G16" s="1">
         <v>0.24018449340550399</v>
       </c>
+      <c r="H16" s="1"/>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>9</v>
       </c>
@@ -8406,8 +8242,9 @@
       <c r="G17" s="1">
         <v>7.7189906228558296E-3</v>
       </c>
+      <c r="H17" s="1"/>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>10</v>
       </c>
@@ -8429,8 +8266,9 @@
       <c r="G18" s="1">
         <v>0.15804746709214099</v>
       </c>
+      <c r="H18" s="1"/>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>10</v>
       </c>
@@ -8452,8 +8290,9 @@
       <c r="G19" s="1">
         <v>6.8448344635021904E-2</v>
       </c>
+      <c r="H19" s="1"/>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>10</v>
       </c>
@@ -8464,7 +8303,7 @@
         <v>1.0346801166138999E-2</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>10</v>
       </c>
@@ -8486,8 +8325,9 @@
       <c r="G21" s="1">
         <v>0.60645193458316704</v>
       </c>
+      <c r="H21" s="1"/>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>10</v>
       </c>
@@ -8509,8 +8349,9 @@
       <c r="G22" s="1">
         <v>9.5253290785799694E-2</v>
       </c>
+      <c r="H22" s="1"/>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>10</v>
       </c>
@@ -8528,8 +8369,9 @@
       <c r="G23" s="1">
         <v>7.1798962903869099E-2</v>
       </c>
+      <c r="H23" s="1"/>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>11</v>
       </c>
@@ -8551,8 +8393,9 @@
       <c r="G24" s="1">
         <v>7.9285722168879399E-2</v>
       </c>
+      <c r="H24" s="1"/>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>11</v>
       </c>
@@ -8574,8 +8417,9 @@
       <c r="G25" s="1">
         <v>6.6362061163902003E-2</v>
       </c>
+      <c r="H25" s="1"/>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>11</v>
       </c>
@@ -8597,8 +8441,9 @@
       <c r="G26" s="1">
         <v>0.44152346897107297</v>
       </c>
+      <c r="H26" s="1"/>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>11</v>
       </c>
@@ -8620,8 +8465,9 @@
       <c r="G27" s="1">
         <v>0.36152037877032001</v>
       </c>
+      <c r="H27" s="1"/>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>11</v>
       </c>
@@ -8643,8 +8489,9 @@
       <c r="G28" s="1">
         <v>5.1308368925824098E-2</v>
       </c>
+      <c r="H28" s="1"/>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>12</v>
       </c>
@@ -8666,8 +8513,9 @@
       <c r="G29" s="1">
         <v>0.106547399807068</v>
       </c>
+      <c r="H29" s="1"/>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>12</v>
       </c>
@@ -8689,8 +8537,9 @@
       <c r="G30" s="1">
         <v>7.75304744365517E-2</v>
       </c>
+      <c r="H30" s="1"/>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>12</v>
       </c>
@@ -8710,8 +8559,9 @@
         <v>1.6368158131458699E-2</v>
       </c>
       <c r="G31" s="1"/>
+      <c r="H31" s="1"/>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>12</v>
       </c>
@@ -8733,8 +8583,9 @@
       <c r="G32" s="1">
         <v>0.49890379724633799</v>
       </c>
+      <c r="H32" s="1"/>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>12</v>
       </c>
@@ -8756,8 +8607,9 @@
       <c r="G33" s="1">
         <v>0.21669034464614501</v>
       </c>
+      <c r="H33" s="1"/>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>12</v>
       </c>
@@ -8779,8 +8631,9 @@
       <c r="G34" s="1">
         <v>0.10032798386389501</v>
       </c>
+      <c r="H34" s="1"/>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>13</v>
       </c>
@@ -8802,8 +8655,9 @@
       <c r="G35" s="1">
         <v>6.2102000337270799E-2</v>
       </c>
+      <c r="H35" s="1"/>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>13</v>
       </c>
@@ -8825,8 +8679,9 @@
       <c r="G36" s="1">
         <v>0.17864513486818301</v>
       </c>
+      <c r="H36" s="1"/>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>13</v>
       </c>
@@ -8846,8 +8701,9 @@
       <c r="G37" s="1">
         <v>7.1662022500782893E-2</v>
       </c>
+      <c r="H37" s="1"/>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>13</v>
       </c>
@@ -8869,8 +8725,9 @@
       <c r="G38" s="1">
         <v>0.33978430726979197</v>
       </c>
+      <c r="H38" s="1"/>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>13</v>
       </c>
@@ -8892,8 +8749,9 @@
       <c r="G39" s="1">
         <v>0.34780653502397002</v>
       </c>
+      <c r="H39" s="1"/>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>13</v>
       </c>
@@ -8907,8 +8765,9 @@
       <c r="E40" s="1"/>
       <c r="F40" s="1"/>
       <c r="G40" s="1"/>
+      <c r="H40" s="1"/>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>14</v>
       </c>
@@ -8930,8 +8789,9 @@
       <c r="G41" s="1">
         <v>0.1040658604998</v>
       </c>
+      <c r="H41" s="1"/>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>14</v>
       </c>
@@ -8953,8 +8813,9 @@
       <c r="G42" s="1">
         <v>9.8803460811646704E-2</v>
       </c>
+      <c r="H42" s="1"/>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>14</v>
       </c>
@@ -8974,8 +8835,9 @@
       <c r="G43" s="1">
         <v>2.95914649130983E-2</v>
       </c>
+      <c r="H43" s="1"/>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>14</v>
       </c>
@@ -8997,8 +8859,9 @@
       <c r="G44" s="1">
         <v>0.35488572711788202</v>
       </c>
+      <c r="H44" s="1"/>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>14</v>
       </c>
@@ -9020,8 +8883,9 @@
       <c r="G45" s="1">
         <v>0.41265348665757101</v>
       </c>
+      <c r="H45" s="1"/>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>14</v>
       </c>
@@ -9035,8 +8899,9 @@
       <c r="E46" s="1"/>
       <c r="F46" s="1"/>
       <c r="G46" s="1"/>
+      <c r="H46" s="1"/>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>15</v>
       </c>
@@ -9058,8 +8923,9 @@
       <c r="G47" s="1">
         <v>0.14308957671415301</v>
       </c>
+      <c r="H47" s="1"/>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>15</v>
       </c>
@@ -9081,8 +8947,9 @@
       <c r="G48" s="1">
         <v>0.136024136517372</v>
       </c>
+      <c r="H48" s="1"/>
     </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>15</v>
       </c>
@@ -9104,8 +8971,9 @@
       <c r="G49" s="1">
         <v>0.50018576406682302</v>
       </c>
+      <c r="H49" s="1"/>
     </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>15</v>
       </c>
@@ -9127,8 +8995,9 @@
       <c r="G50" s="1">
         <v>0.22070052270165</v>
       </c>
+      <c r="H50" s="1"/>
     </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>15</v>
       </c>
@@ -9142,8 +9011,9 @@
         <v>1.3370504394062401E-2</v>
       </c>
       <c r="G51" s="1"/>
+      <c r="H51" s="1"/>
     </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>16</v>
       </c>
@@ -9165,8 +9035,9 @@
       <c r="G52" s="1">
         <v>0.18564347845291301</v>
       </c>
+      <c r="H52" s="1"/>
     </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>16</v>
       </c>
@@ -9188,8 +9059,9 @@
       <c r="G53" s="1">
         <v>8.2178339648595805E-2</v>
       </c>
+      <c r="H53" s="1"/>
     </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>16</v>
       </c>
@@ -9203,8 +9075,9 @@
       </c>
       <c r="F54" s="1"/>
       <c r="G54" s="1"/>
+      <c r="H54" s="1"/>
     </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>16</v>
       </c>
@@ -9226,8 +9099,9 @@
       <c r="G55" s="1">
         <v>0.36535555296144201</v>
       </c>
+      <c r="H55" s="1"/>
     </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>16</v>
       </c>
@@ -9249,8 +9123,9 @@
       <c r="G56" s="1">
         <v>0.35019576788018503</v>
       </c>
+      <c r="H56" s="1"/>
     </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>16</v>
       </c>
@@ -9268,8 +9143,9 @@
       <c r="G57" s="1">
         <v>1.6626861056862601E-2</v>
       </c>
+      <c r="H57" s="1"/>
     </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>17</v>
       </c>
@@ -9291,8 +9167,9 @@
       <c r="G58" s="1">
         <v>7.0547767751324306E-2</v>
       </c>
+      <c r="H58" s="1"/>
     </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>17</v>
       </c>
@@ -9314,8 +9191,9 @@
       <c r="G59" s="1">
         <v>9.2768275002894002E-2</v>
       </c>
+      <c r="H59" s="1"/>
     </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>17</v>
       </c>
@@ -9329,8 +9207,9 @@
       </c>
       <c r="F60" s="1"/>
       <c r="G60" s="1"/>
+      <c r="H60" s="1"/>
     </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>17</v>
       </c>
@@ -9352,8 +9231,9 @@
       <c r="G61" s="1">
         <v>0.51991907788477898</v>
       </c>
+      <c r="H61" s="1"/>
     </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
         <v>17</v>
       </c>
@@ -9375,8 +9255,9 @@
       <c r="G62" s="1">
         <v>0.30195855773418001</v>
       </c>
+      <c r="H62" s="1"/>
     </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
         <v>17</v>
       </c>
@@ -9392,8 +9273,9 @@
       <c r="E63" s="1"/>
       <c r="F63" s="1"/>
       <c r="G63" s="1"/>
+      <c r="H63" s="1"/>
     </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
         <v>17</v>
       </c>
@@ -9411,8 +9293,9 @@
       <c r="G64" s="1">
         <v>1.4806321626821099E-2</v>
       </c>
+      <c r="H64" s="1"/>
     </row>
-    <row r="65" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
         <v>19</v>
       </c>
@@ -9420,22 +9303,29 @@
         <v>5</v>
       </c>
       <c r="C65" s="1">
-        <v>0.18777452415812501</v>
+        <v>0.327897218236407</v>
       </c>
       <c r="D65" s="1">
-        <v>0.13612368024132701</v>
+        <v>0.31179600782962302</v>
       </c>
       <c r="E65" s="1">
-        <v>0.16322701688555299</v>
+        <v>0.26873852467869103</v>
       </c>
       <c r="F65" s="1">
-        <v>0.245287253141831</v>
+        <v>0.26857494312742503</v>
       </c>
       <c r="G65" s="1">
-        <v>0.19667389732465601</v>
+        <v>0.22154317602096299</v>
+      </c>
+      <c r="H65" s="1">
+        <f>I65/I$69</f>
+        <v>0.24257252708843061</v>
+      </c>
+      <c r="I65" s="2">
+        <v>694</v>
       </c>
     </row>
-    <row r="66" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
         <v>19</v>
       </c>
@@ -9443,22 +9333,29 @@
         <v>3</v>
       </c>
       <c r="C66" s="1">
-        <v>6.2957540263543096E-2</v>
+        <v>0.12768138135603399</v>
       </c>
       <c r="D66" s="1">
-        <v>6.4856711915535395E-2</v>
+        <v>0.104387167856347</v>
       </c>
       <c r="E66" s="1">
-        <v>0.113508442776735</v>
+        <v>0.14865266227454299</v>
       </c>
       <c r="F66" s="1">
-        <v>0.12253141831238699</v>
+        <v>0.14582025178337901</v>
       </c>
       <c r="G66" s="1">
-        <v>8.38756326825741E-2</v>
+        <v>0.100751303681649</v>
+      </c>
+      <c r="H66" s="1">
+        <f>I66/I$69</f>
+        <v>7.1303739951066064E-2</v>
+      </c>
+      <c r="I66" s="2">
+        <v>204</v>
       </c>
     </row>
-    <row r="67" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
         <v>19</v>
       </c>
@@ -9466,22 +9363,29 @@
         <v>4</v>
       </c>
       <c r="C67" s="1">
-        <v>0.39677891654465502</v>
+        <v>0.212689761614797</v>
       </c>
       <c r="D67" s="1">
-        <v>0.35105580693815902</v>
+        <v>0.19818441811127899</v>
       </c>
       <c r="E67" s="1">
-        <v>0.297373358348968</v>
+        <v>0.18631871692407301</v>
       </c>
       <c r="F67" s="1">
-        <v>0.24730700179533199</v>
+        <v>0.23762442484070501</v>
       </c>
       <c r="G67" s="1">
-        <v>0.28958785249457702</v>
+        <v>0.26222936091305599</v>
+      </c>
+      <c r="H67" s="1">
+        <f>I67/I$69</f>
+        <v>0.29605033205173015</v>
+      </c>
+      <c r="I67" s="2">
+        <v>847</v>
       </c>
     </row>
-    <row r="68" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
         <v>19</v>
       </c>
@@ -9489,22 +9393,29 @@
         <v>20</v>
       </c>
       <c r="C68" s="1">
-        <v>0.35248901903367402</v>
+        <v>0.33173163879276002</v>
       </c>
       <c r="D68" s="1">
-        <v>0.44796380090497701</v>
+        <v>0.38563240620274902</v>
       </c>
       <c r="E68" s="1">
-        <v>0.42589118198874298</v>
+        <v>0.396290096122691</v>
       </c>
       <c r="F68" s="1">
-        <v>0.337073608617594</v>
+        <v>0.30467744757944099</v>
       </c>
       <c r="G68" s="1">
-        <v>0.42986261749819199</v>
+        <v>0.41547615938433102</v>
+      </c>
+      <c r="H68" s="1">
+        <f>I68/I$69</f>
+        <v>0.39007340090877318</v>
+      </c>
+      <c r="I68" s="2">
+        <v>1116</v>
       </c>
     </row>
-    <row r="69" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
         <v>19</v>
       </c>
@@ -9515,9 +9426,20 @@
       <c r="D69" s="1"/>
       <c r="E69" s="1"/>
       <c r="F69" s="1">
-        <v>4.7800718132854497E-2</v>
+        <v>4.3302932669047903E-2</v>
       </c>
       <c r="G69" s="1"/>
+      <c r="H69" s="1"/>
+      <c r="I69" s="2">
+        <f>SUM(I65:I68)</f>
+        <v>2861</v>
+      </c>
+    </row>
+    <row r="71" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="H71" s="3">
+        <f>((G68-H68)+(H67-G67))/2</f>
+        <v>2.9611864807116001E-2</v>
+      </c>
     </row>
   </sheetData>
   <sortState ref="A2:G69">

</xml_diff>